<commit_message>
corectura cerinte si cod
</commit_message>
<xml_diff>
--- a/Docs/initial/CheckList/Lab01_ReviewReport (version 2).xlsx
+++ b/Docs/initial/CheckList/Lab01_ReviewReport (version 2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\Anul3Sem2\VVSS\Lab\01_Tasks\Docs\initial\CheckList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{855D3078-695F-465E-9F7A-24040FB55D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D5111F4-7156-4979-BA66-BB53CF947751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="88">
   <si>
     <t>do not print this form</t>
   </si>
@@ -120,13 +120,13 @@
     <t>F01</t>
   </si>
   <si>
-    <t>Nu se specifica lungime maxima/minima a descrierii si formatul pentru data si ora.</t>
+    <t>Nu se specifica lungime maxima/minima a descrierii si formatul pentru data si ora</t>
   </si>
   <si>
     <t>R05</t>
   </si>
   <si>
-    <t>Functionalitatea de a seta un interval nu este definita corect deoarece un interval mai mare este greu de inteles si precizat de catre utilizator in ore si minute.</t>
+    <t>detalii legate de interfata nu sunt specificate.</t>
   </si>
   <si>
     <t>Nu se precizeaza cum ne vom da seama daca task-ul este activ sau nu.</t>
@@ -165,6 +165,12 @@
     <t>Detalii legate de interfata nu sunt specificate.</t>
   </si>
   <si>
+    <t>Lipseste atributul de titlu</t>
+  </si>
+  <si>
+    <t>Lipsesc mesajele de in caz de erori</t>
+  </si>
+  <si>
     <t>Effort to review document (hours):</t>
   </si>
   <si>
@@ -207,7 +213,7 @@
     <t>NewEditController</t>
   </si>
   <si>
-    <t>Lipseste modificare listei obsevable</t>
+    <t>Lipseste modificare listei obsevable(pentru add si edit)</t>
   </si>
   <si>
     <t>C01</t>
@@ -253,6 +259,24 @@
   </si>
   <si>
     <t>Clasele nu repsecta niciun fel de regula la aranjarea in fisiere</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>In loc de variabila descriere avem variabila  titlu</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nu sunt puse mesaje de alert in caz ca utilizatorul </t>
+  </si>
+  <si>
+    <t>Apar erori la popup ul cu notificari daca fereastra aplicatiei nu e deschisa</t>
+  </si>
+  <si>
+    <t>Validarile facute in constructor</t>
   </si>
   <si>
     <t>Tool-based Code Analysis</t>
@@ -480,8 +504,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -518,10 +546,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -866,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -887,27 +911,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="34"/>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18" t="s">
         <v>3</v>
@@ -917,13 +941,13 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="18" t="s">
         <v>5</v>
       </c>
@@ -935,17 +959,17 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="18" t="s">
         <v>9</v>
       </c>
@@ -957,17 +981,17 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="18" t="s">
         <v>13</v>
       </c>
@@ -975,39 +999,39 @@
       <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="34"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="34"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
@@ -1020,14 +1044,14 @@
       <c r="E9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="34"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="18">
         <v>1</v>
       </c>
@@ -1040,14 +1064,14 @@
       <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="34"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="18">
         <f>B10+1</f>
         <v>2</v>
@@ -1061,14 +1085,14 @@
       <c r="E11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-    </row>
-    <row r="12" spans="1:10" ht="28.9">
-      <c r="A12" s="34"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" ht="30">
+      <c r="A12" s="21"/>
       <c r="B12" s="18">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1082,14 +1106,14 @@
       <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-    </row>
-    <row r="13" spans="1:10" ht="57.6">
-      <c r="A13" s="34"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" ht="15">
+      <c r="A13" s="21"/>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1103,14 +1127,14 @@
       <c r="E13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="28.9">
-      <c r="A14" s="34"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1124,14 +1148,14 @@
       <c r="E14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="34"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1145,14 +1169,14 @@
       <c r="E15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10" ht="43.15">
-      <c r="A16" s="34"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1166,11 +1190,11 @@
       <c r="E16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:5" ht="28.9">
       <c r="B17" s="18">
@@ -1230,23 +1254,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" ht="15">
       <c r="B21" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-    </row>
-    <row r="22" spans="2:5">
+      <c r="C21" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15">
       <c r="B22" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
+      <c r="E22" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="18">
@@ -1276,15 +1308,15 @@
       <c r="E25" s="19"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="34"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="1"/>
@@ -1330,27 +1362,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="34"/>
-      <c r="B2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18" t="s">
         <v>3</v>
@@ -1360,13 +1392,13 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="18" t="s">
         <v>5</v>
       </c>
@@ -1374,17 +1406,17 @@
       <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="D4" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="18" t="s">
         <v>9</v>
       </c>
@@ -1392,17 +1424,17 @@
       <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
+        <v>48</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="30"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="18" t="s">
         <v>13</v>
       </c>
@@ -1410,35 +1442,35 @@
       <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="34"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="34"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
@@ -1451,28 +1483,28 @@
       <c r="E9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="34"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="18">
         <v>1</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="34"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="18">
         <f>B10+1</f>
         <v>2</v>
@@ -1480,14 +1512,14 @@
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="34"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="18">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1495,14 +1527,14 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="34"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1510,14 +1542,14 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="34"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1525,14 +1557,14 @@
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="34"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1540,14 +1572,14 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="34"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1555,11 +1587,11 @@
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="18">
@@ -1652,15 +1684,15 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="34"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="1"/>
@@ -1686,8 +1718,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1707,27 +1739,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="34"/>
-      <c r="B2" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18" t="s">
         <v>3</v>
@@ -1737,13 +1769,13 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="18" t="s">
         <v>5</v>
       </c>
@@ -1751,17 +1783,17 @@
       <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="D4" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="18" t="s">
         <v>9</v>
       </c>
@@ -1769,17 +1801,17 @@
       <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
+      <c r="D5" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="33"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="18" t="s">
         <v>13</v>
       </c>
@@ -1787,37 +1819,37 @@
       <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="34"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+      <c r="D6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="34"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
@@ -1830,155 +1862,155 @@
       <c r="E9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="34"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="18">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-    </row>
-    <row r="11" spans="1:10" ht="15">
-      <c r="A11" s="34"/>
+        <v>56</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11" spans="1:10" ht="30">
+      <c r="A11" s="21"/>
       <c r="B11" s="18">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+        <v>59</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10" ht="30">
-      <c r="A12" s="34"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="18">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
+        <v>62</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="34"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" ht="30">
+      <c r="A14" s="21"/>
+      <c r="B14" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="30">
+      <c r="A15" s="21"/>
+      <c r="B15" s="18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10" ht="30">
-      <c r="A14" s="34"/>
-      <c r="B14" s="18">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-    </row>
-    <row r="15" spans="1:10" ht="30">
-      <c r="A15" s="34"/>
-      <c r="B15" s="18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
+        <v>69</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10" ht="30">
-      <c r="A16" s="34"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+        <v>71</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:5" ht="30">
       <c r="B17" s="18">
@@ -1986,50 +2018,74 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30">
       <c r="B18" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="30">
       <c r="B19" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5">
+      <c r="C19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="30">
       <c r="B20" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5">
+      <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15">
       <c r="B21" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="18">
@@ -2113,15 +2169,15 @@
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="34"/>
+      <c r="B32" s="21"/>
       <c r="C32" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="1"/>
@@ -2169,27 +2225,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="34"/>
-      <c r="B2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18" t="s">
         <v>3</v>
@@ -2199,13 +2255,13 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="18" t="s">
         <v>5</v>
       </c>
@@ -2213,15 +2269,15 @@
       <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+        <v>82</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="18" t="s">
         <v>9</v>
       </c>
@@ -2229,15 +2285,15 @@
       <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="18" t="s">
         <v>13</v>
       </c>
@@ -2245,43 +2301,43 @@
       <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="34"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="34"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+        <v>86</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="34"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="18">
         <v>1</v>
       </c>
@@ -2289,13 +2345,13 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="34"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="18">
         <f>B10+1</f>
         <v>2</v>
@@ -2304,13 +2360,13 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="34"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="18">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -2319,13 +2375,13 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="34"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2334,13 +2390,13 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="34"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2349,13 +2405,13 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="34"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2364,13 +2420,13 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="34"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2379,10 +2435,10 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="18">
@@ -2525,19 +2581,19 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="2:6">
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="B32" s="34"/>
-      <c r="C32" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="15"/>
     </row>
   </sheetData>

</xml_diff>